<commit_message>
update libre test file
</commit_message>
<xml_diff>
--- a/tests/TestUtils/TestFiles/TestWorkbook_Libre.xlsx
+++ b/tests/TestUtils/TestFiles/TestWorkbook_Libre.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="WithTable" sheetId="1" state="visible" r:id="rId2"/>
@@ -70,8 +70,8 @@
   <numFmts count="4">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="m/d/yyyy"/>
-    <numFmt numFmtId="166" formatCode="General"/>
-    <numFmt numFmtId="167" formatCode="d/m/yy\ h:mm;@"/>
+    <numFmt numFmtId="166" formatCode="d/m/yy\ h:mm;@"/>
+    <numFmt numFmtId="167" formatCode="0.00"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -208,7 +208,7 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E23" activeCellId="0" sqref="E23"/>
+      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.4296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -248,7 +248,7 @@
       <c r="C2" s="2" t="n">
         <v>45213</v>
       </c>
-      <c r="D2" s="3" t="n">
+      <c r="D2" s="0" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -266,10 +266,10 @@
       <c r="B3" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="4" t="n">
+      <c r="C3" s="3" t="n">
         <v>45214.75</v>
       </c>
-      <c r="D3" s="3" t="n">
+      <c r="D3" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -284,17 +284,17 @@
       <c r="B4" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="4" t="n">
+      <c r="C4" s="3" t="n">
         <v>45215.8333333333</v>
       </c>
-      <c r="D4" s="3" t="n">
+      <c r="D4" s="0" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="n">
-        <v>4</v>
+      <c r="A5" s="4" t="n">
+        <v>4.269</v>
       </c>
       <c r="B5" s="0" t="s">
         <v>12</v>
@@ -302,7 +302,7 @@
       <c r="C5" s="2" t="n">
         <v>45216</v>
       </c>
-      <c r="D5" s="3" t="n">
+      <c r="D5" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -328,8 +328,8 @@
   </sheetPr>
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I19" activeCellId="0" sqref="I19"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -368,7 +368,7 @@
       <c r="C2" s="2" t="n">
         <v>45213</v>
       </c>
-      <c r="D2" s="3" t="n">
+      <c r="D2" s="0" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -386,10 +386,10 @@
       <c r="B3" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="4" t="n">
+      <c r="C3" s="3" t="n">
         <v>45214.75</v>
       </c>
-      <c r="D3" s="3" t="n">
+      <c r="D3" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -404,17 +404,17 @@
       <c r="B4" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="4" t="n">
+      <c r="C4" s="3" t="n">
         <v>45215.8333333333</v>
       </c>
-      <c r="D4" s="3" t="n">
+      <c r="D4" s="0" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="n">
-        <v>4</v>
+      <c r="A5" s="4" t="n">
+        <v>4.269</v>
       </c>
       <c r="B5" s="0" t="s">
         <v>12</v>
@@ -422,7 +422,7 @@
       <c r="C5" s="2" t="n">
         <v>45216</v>
       </c>
-      <c r="D5" s="3" t="n">
+      <c r="D5" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -445,8 +445,8 @@
   </sheetPr>
   <dimension ref="B4:G8"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M11" activeCellId="0" sqref="M11"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.4296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -484,7 +484,7 @@
       <c r="D5" s="2" t="n">
         <v>45213</v>
       </c>
-      <c r="E5" s="3" t="n">
+      <c r="E5" s="0" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -502,10 +502,10 @@
       <c r="C6" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="4" t="n">
+      <c r="D6" s="3" t="n">
         <v>45214.75</v>
       </c>
-      <c r="E6" s="3" t="n">
+      <c r="E6" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -520,17 +520,17 @@
       <c r="C7" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="4" t="n">
+      <c r="D7" s="3" t="n">
         <v>45215.8333333333</v>
       </c>
-      <c r="E7" s="3" t="n">
+      <c r="E7" s="0" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="0" t="n">
-        <v>4</v>
+      <c r="B8" s="4" t="n">
+        <v>4.269</v>
       </c>
       <c r="C8" s="0" t="s">
         <v>12</v>
@@ -538,7 +538,7 @@
       <c r="D8" s="2" t="n">
         <v>45216</v>
       </c>
-      <c r="E8" s="3" t="n">
+      <c r="E8" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>

</xml_diff>